<commit_message>
orcuttieae and sanicula alignments
</commit_message>
<xml_diff>
--- a/fine-scale/lineages_for_analyses.xlsx
+++ b/fine-scale/lineages_for_analyses.xlsx
@@ -937,7 +937,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1062,6 +1062,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2552,7 +2555,9 @@
       <c r="O4" t="s" s="22">
         <v>30</v>
       </c>
-      <c r="P4" s="19"/>
+      <c r="P4" t="s" s="22">
+        <v>30</v>
+      </c>
       <c r="Q4" s="19"/>
       <c r="R4" t="s" s="18">
         <v>31</v>
@@ -3011,7 +3016,9 @@
       <c r="O13" t="s" s="22">
         <v>30</v>
       </c>
-      <c r="P13" s="19"/>
+      <c r="P13" t="s" s="22">
+        <v>30</v>
+      </c>
       <c r="Q13" s="19"/>
       <c r="R13" t="s" s="18">
         <v>80</v>
@@ -3853,14 +3860,22 @@
       <c r="N30" t="s" s="21">
         <v>30</v>
       </c>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
+      <c r="O30" t="s" s="22">
+        <v>30</v>
+      </c>
+      <c r="P30" t="s" s="22">
+        <v>30</v>
+      </c>
       <c r="Q30" s="19"/>
       <c r="R30" t="s" s="18">
         <v>168</v>
       </c>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
+      <c r="S30" s="19">
+        <v>54</v>
+      </c>
+      <c r="T30" s="19">
+        <v>633</v>
+      </c>
       <c r="U30" t="s" s="18">
         <v>59</v>
       </c>
@@ -4433,14 +4448,22 @@
       <c r="N42" t="s" s="41">
         <v>30</v>
       </c>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
+      <c r="O42" t="s" s="42">
+        <v>30</v>
+      </c>
+      <c r="P42" t="s" s="42">
+        <v>30</v>
+      </c>
       <c r="Q42" s="39"/>
       <c r="R42" t="s" s="38">
         <v>216</v>
       </c>
-      <c r="S42" s="39"/>
-      <c r="T42" s="39"/>
+      <c r="S42" s="39">
+        <v>41</v>
+      </c>
+      <c r="T42" s="39">
+        <v>1136</v>
+      </c>
       <c r="U42" t="s" s="38">
         <v>219</v>
       </c>
@@ -4451,7 +4474,7 @@
       <c r="X42" s="39"/>
       <c r="Y42" s="39"/>
       <c r="Z42" s="39"/>
-      <c r="AA42" s="42"/>
+      <c r="AA42" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4473,12 +4496,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="43" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="43" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="43" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="43" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="43" customWidth="1"/>
-    <col min="6" max="256" width="10.875" style="43" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="44" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="44" customWidth="1"/>
+    <col min="6" max="256" width="10.875" style="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.65" customHeight="1">

</xml_diff>